<commit_message>
public/listo-cargas.xlsx => datos de prueba resources/views/mails/mailsLoads.blade.php => ajuste en ruta de consulta del certificado
</commit_message>
<xml_diff>
--- a/public/listo-cargas.xlsx
+++ b/public/listo-cargas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CursosCertificados\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8A72B2-34A7-493D-87DA-B39403CD1C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E833D65-22BC-4418-B6CC-DFE120EE1DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{89225295-1B4F-4398-8825-9DC914083096}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89225295-1B4F-4398-8825-9DC914083096}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="6" r:id="rId1"/>
@@ -36,47 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
-  <si>
-    <t>Olivia Montes Segundo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Estudiante</t>
   </si>
   <si>
-    <t>rodrigo.saul@example.com</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>Curso de diseño de HV</t>
-  </si>
-  <si>
     <t>Presencial</t>
   </si>
   <si>
-    <t>Bogotá</t>
-  </si>
-  <si>
-    <t>Sra. Valeria Clemente</t>
-  </si>
-  <si>
-    <t>manuel.zamora@example.net</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
-    <t>Curso de empleabilidad</t>
-  </si>
-  <si>
-    <t>2023/05/11</t>
-  </si>
-  <si>
-    <t>2023/05/12</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -105,6 +75,63 @@
   </si>
   <si>
     <t>ciudad_expedicion</t>
+  </si>
+  <si>
+    <t>jack sebastian murillo salamanca</t>
+  </si>
+  <si>
+    <t>jack_murillo@cun.edu.co</t>
+  </si>
+  <si>
+    <t>Curso de ortografia</t>
+  </si>
+  <si>
+    <t>virtual</t>
+  </si>
+  <si>
+    <t>Bogota</t>
+  </si>
+  <si>
+    <t>johan camilo triana avendaño</t>
+  </si>
+  <si>
+    <t>johan_trianaa@cun.edu.co</t>
+  </si>
+  <si>
+    <t>nelson_cardenas@cun.edu.co</t>
+  </si>
+  <si>
+    <t>nelson andres cardenas velasquez</t>
+  </si>
+  <si>
+    <t>Estudiantes</t>
+  </si>
+  <si>
+    <t>gabriel_pirela@cun.edu.co</t>
+  </si>
+  <si>
+    <t>gabriel alfonso pirela jaramillo</t>
+  </si>
+  <si>
+    <t>2023-06-07</t>
+  </si>
+  <si>
+    <t>hamer_forero@cun.edu.co</t>
+  </si>
+  <si>
+    <t>hamer fernando forero ruiz</t>
+  </si>
+  <si>
+    <t>sonia_acosta@cun.edu.co</t>
+  </si>
+  <si>
+    <t>sonia mireya acosta lopez</t>
+  </si>
+  <si>
+    <t>brian steven cañon rojas</t>
+  </si>
+  <si>
+    <t>brian_canon@cun.edu.co</t>
   </si>
 </sst>
 </file>
@@ -463,108 +490,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C3A0C-7E08-4CC4-8411-0CE9730A587C}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>123456701</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>123456702</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>123456703</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>123456704</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>19905020</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
+      <c r="E6">
+        <v>123456705</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>123456706</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>45</v>
+      </c>
+      <c r="I7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>59651840</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>123456707</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustes para envio de correo en cola
</commit_message>
<xml_diff>
--- a/public/listo-cargas.xlsx
+++ b/public/listo-cargas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CursosCertificados\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E833D65-22BC-4418-B6CC-DFE120EE1DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79083A74-07A1-4AB8-955D-D34FD66AC581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89225295-1B4F-4398-8825-9DC914083096}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>Estudiante</t>
   </si>
@@ -132,13 +132,19 @@
   </si>
   <si>
     <t>brian_canon@cun.edu.co</t>
+  </si>
+  <si>
+    <t>janluy moreno</t>
+  </si>
+  <si>
+    <t>janluy_moreno@cun.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +154,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,14 +184,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341C3A0C-7E08-4CC4-8411-0CE9730A587C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H9" sqref="H9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,8 +771,43 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1022348425</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{BF6D1372-3630-4E3F-A8FE-09623E9C50A8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>